<commit_message>
Tested test cases for SP2_US8 as tester 2
</commit_message>
<xml_diff>
--- a/Testing/Testing 1.xlsx
+++ b/Testing/Testing 1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ganga\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aneesh Dalvi\Desktop\new\Breitenburg-SER515\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CECBF7AB-5A7F-43E3-ACE1-DCFC74DDC1E6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -116,7 +115,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -306,23 +305,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -358,23 +340,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -550,32 +515,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="90" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="93.75" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -601,7 +566,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -618,10 +583,12 @@
         <v>6</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="G4" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -638,10 +605,12 @@
         <v>6</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="G5" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>3</v>
       </c>
@@ -658,10 +627,12 @@
         <v>6</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="G6" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>4</v>
       </c>
@@ -678,10 +649,12 @@
         <v>6</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="G7" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>5</v>
       </c>
@@ -700,10 +673,12 @@
       <c r="F8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="4"/>
+      <c r="G8" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>6</v>
       </c>
@@ -720,10 +695,12 @@
         <v>6</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="G9" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>7</v>
       </c>
@@ -740,7 +717,9 @@
         <v>6</v>
       </c>
       <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="G10" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="H10" s="4"/>
     </row>
   </sheetData>
@@ -750,24 +729,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added changes to the testing1 document
</commit_message>
<xml_diff>
--- a/Testing/Testing 1.xlsx
+++ b/Testing/Testing 1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -110,6 +110,9 @@
 Test Case created : 10/14/2018
 Test Case review : 10/14/2018
 Linked User Story : 8 and 12</t>
+  </si>
+  <si>
+    <t>Aneesh Dalvi</t>
   </si>
 </sst>
 </file>
@@ -518,7 +521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -583,10 +586,12 @@
         <v>6</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="4"/>
+      <c r="G4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -605,10 +610,12 @@
         <v>6</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -627,10 +634,12 @@
         <v>6</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -649,10 +658,12 @@
         <v>6</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
@@ -673,10 +684,12 @@
       <c r="F8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -695,10 +708,12 @@
         <v>6</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="4"/>
+      <c r="G9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -717,10 +732,12 @@
         <v>6</v>
       </c>
       <c r="F10" s="4"/>
-      <c r="G10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="4"/>
+      <c r="G10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>